<commit_message>
Fix small / regular cpu inversion
</commit_message>
<xml_diff>
--- a/docs/policies/2022_ULHPC_Usage_Charging.xlsx
+++ b/docs/policies/2022_ULHPC_Usage_Charging.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jschleich/git/github.com/ULHPC/ulhpc-docs/docs/policies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F3A1D4-6A0D-C14A-AA75-AE0F2E1A99F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811FDB4E-F5C9-6844-A921-CE603BE48134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimates based on funded PM" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -530,23 +530,20 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -563,49 +560,53 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,7 +827,7 @@
   </sheetPr>
   <dimension ref="A1:AE1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -884,13 +885,13 @@
     </row>
     <row r="2" spans="1:31" ht="33.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -919,7 +920,7 @@
     </row>
     <row r="3" spans="1:31" ht="32.25" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="67" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="38"/>
@@ -954,13 +955,13 @@
     </row>
     <row r="4" spans="1:31" ht="13">
       <c r="A4" s="1"/>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="68" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
-      <c r="F4" s="50"/>
+      <c r="F4" s="69"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -969,7 +970,7 @@
     </row>
     <row r="5" spans="1:31" ht="33" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="67" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="38"/>
@@ -983,13 +984,13 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:31" ht="13">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="70" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="50"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1000,13 +1001,13 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:31" ht="13">
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="44"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="53"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1032,13 +1033,13 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:31" ht="30.75" customHeight="1">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1069,12 +1070,12 @@
       <c r="B11" s="9">
         <v>5529.6</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1102,13 +1103,13 @@
     </row>
     <row r="13" spans="1:31" ht="31.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="62"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1123,7 +1124,7 @@
       <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="62">
+      <c r="C14" s="63">
         <f>SUM(C19:C81)</f>
         <v>60</v>
       </c>
@@ -1161,13 +1162,13 @@
       <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="63">
+      <c r="C15" s="44">
         <f>SUM(D19:D81)</f>
         <v>27648.000000000004</v>
       </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="65"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
       <c r="G15" s="1"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -1192,13 +1193,13 @@
     </row>
     <row r="17" spans="1:14" ht="31.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="68"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
       <c r="G17" s="1"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -1215,7 +1216,7 @@
       <c r="C18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="69" t="s">
+      <c r="D18" s="50" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="38"/>
@@ -1229,7 +1230,7 @@
       <c r="C19" s="18">
         <v>12</v>
       </c>
-      <c r="D19" s="70">
+      <c r="D19" s="42">
         <f t="shared" ref="D19:D81" si="0">IF($B$11*(C19/12)=0,"",$B$11*(C19/12))</f>
         <v>5529.6</v>
       </c>
@@ -1244,7 +1245,7 @@
       <c r="C20" s="7">
         <v>24</v>
       </c>
-      <c r="D20" s="71">
+      <c r="D20" s="43">
         <f t="shared" si="0"/>
         <v>11059.2</v>
       </c>
@@ -1258,7 +1259,7 @@
       <c r="C21" s="18">
         <v>18</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="42">
         <f t="shared" si="0"/>
         <v>8294.4000000000015</v>
       </c>
@@ -1272,7 +1273,7 @@
       <c r="C22" s="7">
         <v>6</v>
       </c>
-      <c r="D22" s="71">
+      <c r="D22" s="43">
         <f t="shared" si="0"/>
         <v>2764.8</v>
       </c>
@@ -1825,12 +1826,12 @@
     <row r="76" spans="2:6" ht="15.75" customHeight="1">
       <c r="B76" s="20"/>
       <c r="C76" s="21"/>
-      <c r="D76" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E76" s="43"/>
-      <c r="F76" s="44"/>
+      <c r="D76" s="71" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E76" s="52"/>
+      <c r="F76" s="53"/>
     </row>
     <row r="77" spans="2:6" ht="15.75" customHeight="1">
       <c r="D77" s="1" t="str">
@@ -2790,60 +2791,11 @@
     <row r="1007" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
     <mergeCell ref="D60:F60"/>
     <mergeCell ref="D61:F61"/>
     <mergeCell ref="D69:F69"/>
@@ -2856,11 +2808,60 @@
     <mergeCell ref="D66:F66"/>
     <mergeCell ref="D67:F67"/>
     <mergeCell ref="D68:F68"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2874,8 +2875,8 @@
   </sheetPr>
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -2894,20 +2895,20 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="35.25" customHeight="1">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="22.5" customHeight="1">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="67" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="38"/>
@@ -2920,13 +2921,13 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="13">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="70" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
-      <c r="F4" s="50"/>
+      <c r="F4" s="69"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2934,7 +2935,7 @@
     </row>
     <row r="5" spans="1:10" ht="13">
       <c r="A5" s="22"/>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="75" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="38"/>
@@ -2948,13 +2949,13 @@
     </row>
     <row r="6" spans="1:10" ht="25.5" customHeight="1">
       <c r="A6" s="22"/>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="78" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="50"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -2962,13 +2963,13 @@
     </row>
     <row r="7" spans="1:10" ht="13">
       <c r="A7" s="22"/>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="44"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="53"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -2988,13 +2989,13 @@
     </row>
     <row r="9" spans="1:10" ht="34.5" customHeight="1">
       <c r="A9" s="22"/>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -3002,7 +3003,7 @@
     </row>
     <row r="10" spans="1:10" ht="13">
       <c r="A10" s="22"/>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="75" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="38"/>
@@ -3015,21 +3016,21 @@
       <c r="C11" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="76" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="38"/>
-      <c r="F11" s="84"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:10" ht="13">
       <c r="B12" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="26">
-        <v>1.25</v>
-      </c>
-      <c r="D12" s="85" t="s">
+      <c r="C12" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="77" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="38"/>
@@ -3041,13 +3042,13 @@
         <v>28</v>
       </c>
       <c r="C13" s="28">
-        <v>0.25</v>
-      </c>
-      <c r="D13" s="86" t="s">
+        <v>1.25</v>
+      </c>
+      <c r="D13" s="72" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="38"/>
-      <c r="F13" s="84"/>
+      <c r="F13" s="73"/>
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="13">
@@ -3057,7 +3058,7 @@
       <c r="C14" s="26">
         <v>6</v>
       </c>
-      <c r="D14" s="85" t="s">
+      <c r="D14" s="77" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="38"/>
@@ -3071,11 +3072,11 @@
       <c r="C15" s="28">
         <v>5</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="72" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="38"/>
-      <c r="F15" s="84"/>
+      <c r="F15" s="73"/>
     </row>
     <row r="16" spans="1:10" ht="13">
       <c r="B16" s="30" t="s">
@@ -3084,11 +3085,11 @@
       <c r="C16" s="31">
         <v>0.02</v>
       </c>
-      <c r="D16" s="87" t="s">
+      <c r="D16" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="53"/>
     </row>
     <row r="17" spans="1:8" ht="13">
       <c r="B17" s="1"/>
@@ -3098,19 +3099,19 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="33.75" customHeight="1">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="62"/>
     </row>
     <row r="19" spans="1:8" ht="13">
       <c r="B19" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="74">
+      <c r="C19" s="82">
         <f>SUM(E25:F28)</f>
         <v>0</v>
       </c>
@@ -3123,13 +3124,13 @@
       <c r="B20" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="77">
+      <c r="C20" s="83">
         <f>SUM(E30)</f>
         <v>0</v>
       </c>
       <c r="D20" s="38"/>
       <c r="E20" s="38"/>
-      <c r="F20" s="78"/>
+      <c r="F20" s="84"/>
       <c r="G20" s="12"/>
       <c r="H20" s="1"/>
     </row>
@@ -3137,13 +3138,13 @@
       <c r="B21" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="79">
+      <c r="C21" s="85">
         <f>SUM(C19:F20)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="53"/>
       <c r="G21" s="12"/>
       <c r="H21" s="1"/>
     </row>
@@ -3152,13 +3153,13 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="34.5" customHeight="1">
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="68"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="49"/>
     </row>
     <row r="24" spans="1:8" ht="28.5" customHeight="1">
       <c r="B24" s="3" t="s">
@@ -3167,7 +3168,7 @@
       <c r="C24" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="76" t="s">
+      <c r="E24" s="80" t="s">
         <v>37</v>
       </c>
       <c r="F24" s="41"/>
@@ -3181,11 +3182,11 @@
       <c r="D25" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="75" t="str">
-        <f t="shared" ref="E25:E28" si="0">IF(C25*C12=0,"",C25*C12)</f>
-        <v/>
-      </c>
-      <c r="F25" s="39"/>
+      <c r="E25" s="81" t="str">
+        <f>IF(C26*C12=0,"",C26*C12)</f>
+        <v/>
+      </c>
+      <c r="F25" s="88"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:8" ht="13">
@@ -3196,8 +3197,8 @@
       <c r="D26" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="74" t="str">
-        <f t="shared" si="0"/>
+      <c r="E26" s="82" t="str">
+        <f>IF(C26*C13=0,"",C26*C13)</f>
         <v/>
       </c>
       <c r="F26" s="41"/>
@@ -3211,8 +3212,8 @@
       <c r="D27" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="75" t="str">
-        <f t="shared" si="0"/>
+      <c r="E27" s="81" t="str">
+        <f t="shared" ref="E25:E28" si="0">IF(C27*C14=0,"",C27*C14)</f>
         <v/>
       </c>
       <c r="F27" s="39"/>
@@ -3227,7 +3228,7 @@
       <c r="D28" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="74" t="str">
+      <c r="E28" s="82" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3243,7 +3244,7 @@
       <c r="D29" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="72" t="s">
+      <c r="E29" s="86" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="39"/>
@@ -3254,11 +3255,11 @@
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
-      <c r="E30" s="73" t="str">
+      <c r="E30" s="87" t="str">
         <f>IF(C30&lt;=1,"",(C30-1)*D30*1024*C16)</f>
         <v/>
       </c>
-      <c r="F30" s="44"/>
+      <c r="F30" s="53"/>
     </row>
     <row r="31" spans="1:8" ht="13">
       <c r="A31" s="1"/>
@@ -3322,6 +3323,18 @@
     <row r="82" ht="13"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="B23:F23"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="B9:F9"/>
@@ -3336,18 +3349,6 @@
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B3:F3"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>